<commit_message>
bj: update sch_sth ia form
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Benin/2024/bj_sch_sth_impact_202401_3_kato_katz_v1.xlsx
+++ b/SCH-STH/Impact assessments/Benin/2024/bj_sch_sth_impact_202401_3_kato_katz_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Benin\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0275A53-B5E4-44F4-A4DA-38CADA48E23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDDD356-9424-4E89-B333-0DD6FCCEC9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>Code d'identification du répondant (Veuillez Saisir le code du participant tel qu'il a été généré dans le formulaire 2)</t>
   </si>
   <si>
-    <t>regex(.,'^[0-9]{3}-[0-9]{2}$')</t>
-  </si>
-  <si>
     <t>k_site_code</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>k_recorder</t>
   </si>
   <si>
-    <t>Veuillez entrer le code du participant. Exemple 123-01</t>
-  </si>
-  <si>
     <t>k_sch_man_sb</t>
   </si>
   <si>
@@ -297,12 +291,6 @@
     <t>C3</t>
   </si>
   <si>
-    <t>Résultats</t>
-  </si>
-  <si>
-    <t>bj_k2</t>
-  </si>
-  <si>
     <t>join(' ', ${k_espen_code_id})</t>
   </si>
   <si>
@@ -312,12 +300,6 @@
     <t>end repeat</t>
   </si>
   <si>
-    <t>(2024 Janvier) - 3. SCH/STH - Kato Katz V3.2</t>
-  </si>
-  <si>
-    <t>bj_sch_sth_impact_202401_3_kato_katz_v3_2</t>
-  </si>
-  <si>
     <t>k_add_record</t>
   </si>
   <si>
@@ -328,6 +310,24 @@
   </si>
   <si>
     <t>select_one yesNo</t>
+  </si>
+  <si>
+    <t>bj_k2_2</t>
+  </si>
+  <si>
+    <t>(2024 Janvier) - 3. SCH/STH - Kato Katz V3.3</t>
+  </si>
+  <si>
+    <t>bj_sch_sth_impact_202401_3_kato_katz_v3_3</t>
+  </si>
+  <si>
+    <t>Cet identifiant est déjà utilisé</t>
+  </si>
+  <si>
+    <t>not(selected(${C3}, ${k_espen_code_id}))</t>
+  </si>
+  <si>
+    <t>Résultats KK</t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -943,20 +943,20 @@
         <v>13</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>54</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>56</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -974,7 +974,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="8"/>
@@ -996,7 +996,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="8"/>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1">
@@ -1020,7 +1020,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="8"/>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="16" customFormat="1">
@@ -1041,10 +1041,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="8"/>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="16" customFormat="1">
@@ -1076,10 +1076,10 @@
     </row>
     <row r="8" spans="1:12" s="16" customFormat="1" ht="47.25">
       <c r="A8" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -1088,18 +1088,18 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="32" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="16" customFormat="1">
       <c r="A9" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="8"/>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="10" spans="1:12" s="16" customFormat="1">
       <c r="A10" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
@@ -1122,15 +1122,15 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="16" customFormat="1" ht="78.75">
       <c r="A11" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -1139,7 +1139,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="16" customFormat="1">
@@ -1155,13 +1155,13 @@
     </row>
     <row r="13" spans="1:12" s="16" customFormat="1">
       <c r="A13" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="8"/>
@@ -1175,23 +1175,23 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="7" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8" t="s">
@@ -1208,14 +1208,14 @@
         <v>19</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="29"/>
       <c r="F15" s="9"/>
       <c r="G15" s="31"/>
       <c r="H15" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I15" s="29"/>
       <c r="J15" s="9" t="s">
@@ -1229,17 +1229,17 @@
         <v>18</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="29"/>
       <c r="F16" s="9"/>
       <c r="G16" s="31"/>
       <c r="H16" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I16" s="29"/>
       <c r="J16" s="9" t="s">
@@ -1253,17 +1253,17 @@
         <v>18</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="29"/>
       <c r="F17" s="9"/>
       <c r="G17" s="31"/>
       <c r="H17" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="9"/>
@@ -1278,14 +1278,14 @@
         <v>20</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="29"/>
       <c r="F18" s="9"/>
       <c r="G18" s="31"/>
       <c r="H18" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I18" s="29"/>
       <c r="J18" s="9" t="s">
@@ -1299,17 +1299,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="35" t="s">
         <v>66</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>68</v>
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="29"/>
       <c r="F19" s="9"/>
       <c r="G19" s="31"/>
       <c r="H19" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I19" s="29"/>
       <c r="J19" s="9" t="s">
@@ -1323,17 +1323,17 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="29"/>
       <c r="F20" s="9"/>
       <c r="G20" s="31"/>
       <c r="H20" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="9"/>
@@ -1348,14 +1348,14 @@
         <v>21</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="29"/>
       <c r="F21" s="9"/>
       <c r="G21" s="31"/>
       <c r="H21" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="9" t="s">
@@ -1369,17 +1369,17 @@
         <v>18</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="29"/>
       <c r="F22" s="9"/>
       <c r="G22" s="31"/>
       <c r="H22" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I22" s="29"/>
       <c r="J22" s="9" t="s">
@@ -1393,17 +1393,17 @@
         <v>18</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="29"/>
       <c r="F23" s="9"/>
       <c r="G23" s="31"/>
       <c r="H23" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I23" s="29"/>
       <c r="J23" s="9"/>
@@ -1418,14 +1418,14 @@
         <v>22</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="29"/>
       <c r="F24" s="9"/>
       <c r="G24" s="31"/>
       <c r="H24" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I24" s="29"/>
       <c r="J24" s="9" t="s">
@@ -1439,17 +1439,17 @@
         <v>18</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="29"/>
       <c r="F25" s="9"/>
       <c r="G25" s="31"/>
       <c r="H25" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="9" t="s">
@@ -1463,17 +1463,17 @@
         <v>18</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="29"/>
       <c r="F26" s="9"/>
       <c r="G26" s="31"/>
       <c r="H26" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I26" s="29"/>
       <c r="J26" s="9"/>
@@ -1488,14 +1488,14 @@
         <v>23</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="29"/>
       <c r="F27" s="9"/>
       <c r="G27" s="31"/>
       <c r="H27" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I27" s="29"/>
       <c r="J27" s="9" t="s">
@@ -1507,17 +1507,17 @@
         <v>18</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="29"/>
       <c r="F28" s="9"/>
       <c r="G28" s="31"/>
       <c r="H28" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I28" s="29"/>
       <c r="J28" s="9" t="s">
@@ -1529,17 +1529,17 @@
         <v>18</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="29"/>
       <c r="F29" s="9"/>
       <c r="G29" s="31"/>
       <c r="H29" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I29" s="29"/>
       <c r="J29" s="4"/>
@@ -1559,7 +1559,7 @@
       <c r="F30" s="24"/>
       <c r="G30" s="11"/>
       <c r="H30" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="9"/>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="30"/>
@@ -1652,16 +1652,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1772,7 +1772,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1794,10 +1794,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="33" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
bj : update forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Benin/2024/bj_sch_sth_impact_202401_3_kato_katz_v1.xlsx
+++ b/SCH-STH/Impact assessments/Benin/2024/bj_sch_sth_impact_202401_3_kato_katz_v1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Benin\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TFGH-WHO\BENIN\SCH STH Janv 2024\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDDD356-9424-4E89-B333-0DD6FCCEC9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="3120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
   <si>
     <t>type</t>
   </si>
@@ -93,9 +92,6 @@
     <t>k_trichuris_sa</t>
   </si>
   <si>
-    <t>k_sch_hae_sa</t>
-  </si>
-  <si>
     <t>k_remarks</t>
   </si>
   <si>
@@ -213,9 +209,6 @@
     <t>Trichocéphale trichura - Lame A</t>
   </si>
   <si>
-    <t>Schistosoma haematobium - Lame A</t>
-  </si>
-  <si>
     <t>k_ascaris_lumb_sb</t>
   </si>
   <si>
@@ -228,18 +221,12 @@
     <t>Trichocéphale trichura - Lame B</t>
   </si>
   <si>
-    <t>Schistosoma haematobium - Lame B</t>
-  </si>
-  <si>
     <t>k_hookworm_sb</t>
   </si>
   <si>
     <t>k_trichuris_sb</t>
   </si>
   <si>
-    <t>k_sch_hae_sb</t>
-  </si>
-  <si>
     <t>Ankylostome - Lame B</t>
   </si>
   <si>
@@ -252,9 +239,6 @@
     <t>k_trichuris_sup</t>
   </si>
   <si>
-    <t>k_sch_hae_sup</t>
-  </si>
-  <si>
     <t>Schistosoma mansoni (nombre d'œufs) - Superviseur</t>
   </si>
   <si>
@@ -267,9 +251,6 @@
     <t>Trichocéphale trichura - Superviseur</t>
   </si>
   <si>
-    <t>Schistosoma haematobium - Superviseur</t>
-  </si>
-  <si>
     <t>Entrez le code de l'enfant exactement tel qu'il a été généré dans le formulaire 2. Exemple: 999-99</t>
   </si>
   <si>
@@ -315,12 +296,6 @@
     <t>bj_k2_2</t>
   </si>
   <si>
-    <t>(2024 Janvier) - 3. SCH/STH - Kato Katz V3.3</t>
-  </si>
-  <si>
-    <t>bj_sch_sth_impact_202401_3_kato_katz_v3_3</t>
-  </si>
-  <si>
     <t>Cet identifiant est déjà utilisé</t>
   </si>
   <si>
@@ -328,12 +303,18 @@
   </si>
   <si>
     <t>Résultats KK</t>
+  </si>
+  <si>
+    <t>bj_sch_sth_impact_202401_3_kato_katz_v4</t>
+  </si>
+  <si>
+    <t>(2024 Janvier) - 3. SCH/STH - Kato Katz V4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -874,14 +855,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -943,20 +924,20 @@
         <v>13</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>52</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>53</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>54</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>55</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -974,7 +955,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="8"/>
@@ -996,7 +977,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="8"/>
@@ -1009,7 +990,7 @@
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1">
@@ -1020,7 +1001,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="8"/>
@@ -1033,7 +1014,7 @@
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="16" customFormat="1">
@@ -1041,10 +1022,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="8"/>
@@ -1057,7 +1038,7 @@
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="16" customFormat="1">
@@ -1076,10 +1057,10 @@
     </row>
     <row r="8" spans="1:12" s="16" customFormat="1" ht="47.25">
       <c r="A8" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -1088,18 +1069,18 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="16" customFormat="1">
       <c r="A9" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="8"/>
@@ -1110,10 +1091,10 @@
     </row>
     <row r="10" spans="1:12" s="16" customFormat="1">
       <c r="A10" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
@@ -1122,15 +1103,15 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="32" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="16" customFormat="1" ht="78.75">
       <c r="A11" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -1139,7 +1120,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="32" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="16" customFormat="1">
@@ -1155,13 +1136,13 @@
     </row>
     <row r="13" spans="1:12" s="16" customFormat="1">
       <c r="A13" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="8"/>
@@ -1175,23 +1156,23 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8" t="s">
@@ -1208,14 +1189,14 @@
         <v>19</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="29"/>
       <c r="F15" s="9"/>
       <c r="G15" s="31"/>
       <c r="H15" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I15" s="29"/>
       <c r="J15" s="9" t="s">
@@ -1229,17 +1210,17 @@
         <v>18</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="29"/>
       <c r="F16" s="9"/>
       <c r="G16" s="31"/>
       <c r="H16" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I16" s="29"/>
       <c r="J16" s="9" t="s">
@@ -1253,17 +1234,17 @@
         <v>18</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="29"/>
       <c r="F17" s="9"/>
       <c r="G17" s="31"/>
       <c r="H17" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="9"/>
@@ -1278,14 +1259,14 @@
         <v>20</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="29"/>
       <c r="F18" s="9"/>
       <c r="G18" s="31"/>
       <c r="H18" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I18" s="29"/>
       <c r="J18" s="9" t="s">
@@ -1299,17 +1280,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="35" t="s">
         <v>64</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>66</v>
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="29"/>
       <c r="F19" s="9"/>
       <c r="G19" s="31"/>
       <c r="H19" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I19" s="29"/>
       <c r="J19" s="9" t="s">
@@ -1323,17 +1304,17 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="35" t="s">
         <v>73</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>78</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="29"/>
       <c r="F20" s="9"/>
       <c r="G20" s="31"/>
       <c r="H20" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="9"/>
@@ -1348,14 +1329,14 @@
         <v>21</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="29"/>
       <c r="F21" s="9"/>
       <c r="G21" s="31"/>
       <c r="H21" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="9" t="s">
@@ -1369,17 +1350,17 @@
         <v>18</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="29"/>
       <c r="F22" s="9"/>
       <c r="G22" s="31"/>
       <c r="H22" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I22" s="29"/>
       <c r="J22" s="9" t="s">
@@ -1393,17 +1374,17 @@
         <v>18</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>74</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>79</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="29"/>
       <c r="F23" s="9"/>
       <c r="G23" s="31"/>
       <c r="H23" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I23" s="29"/>
       <c r="J23" s="9"/>
@@ -1418,14 +1399,14 @@
         <v>22</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="29"/>
       <c r="F24" s="9"/>
       <c r="G24" s="31"/>
       <c r="H24" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I24" s="29"/>
       <c r="J24" s="9" t="s">
@@ -1439,17 +1420,17 @@
         <v>18</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="29"/>
       <c r="F25" s="9"/>
       <c r="G25" s="31"/>
       <c r="H25" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="9" t="s">
@@ -1463,160 +1444,96 @@
         <v>18</v>
       </c>
       <c r="B26" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="36" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>80</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="29"/>
       <c r="F26" s="9"/>
       <c r="G26" s="31"/>
       <c r="H26" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I26" s="29"/>
       <c r="J26" s="9"/>
       <c r="K26" s="29"/>
       <c r="L26" s="29"/>
     </row>
-    <row r="27" spans="1:12" s="17" customFormat="1">
+    <row r="27" spans="1:12">
       <c r="A27" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>63</v>
+      <c r="C27" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="D27" s="11"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="31"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I27" s="29"/>
-      <c r="J27" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="17" customFormat="1">
+        <v>88</v>
+      </c>
+      <c r="I27" s="10"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>68</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I28" s="29"/>
-      <c r="J28" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="17" customFormat="1">
+      <c r="E28" s="10"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>81</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C29" s="30"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I29" s="29"/>
-      <c r="J29" s="4"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="9" t="s">
-        <v>17</v>
+      <c r="A30" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>25</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C30" s="30"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
       <c r="F30" s="24"/>
       <c r="G30" s="11"/>
-      <c r="H30" s="8" t="s">
-        <v>94</v>
-      </c>
+      <c r="H30" s="29"/>
       <c r="I30" s="10"/>
       <c r="J30" s="9"/>
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1625,7 +1542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1643,7 +1560,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -1652,38 +1569,38 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="C2" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1768,11 +1685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1783,24 +1700,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>